<commit_message>
Again increasing allowed spillage, adding lower balance penalty to steam, hydro, and heat nodes, removing dummy variables from unit minimum generation equations.
</commit_message>
<xml_diff>
--- a/src_files/data_files/industrialCHP.xlsx
+++ b/src_files/data_files/industrialCHP.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBFAD02-ED28-4D74-AFBF-9D9EAE2A31BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4323FB8-F312-4A27-973F-DD0071731573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="799" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="799" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitdata" sheetId="8" r:id="rId1"/>
     <sheet name="remove_units" sheetId="9" r:id="rId2"/>
     <sheet name="demanddata" sheetId="7" r:id="rId3"/>
-    <sheet name="Summary" sheetId="4" r:id="rId4"/>
-    <sheet name="H2Heavy, capacities" sheetId="1" r:id="rId5"/>
-    <sheet name="H2Heavy, demands" sheetId="2" r:id="rId6"/>
-    <sheet name="TYNDP2024" sheetId="6" r:id="rId7"/>
-    <sheet name="Eurostat" sheetId="5" r:id="rId8"/>
-    <sheet name="source" sheetId="3" r:id="rId9"/>
+    <sheet name="storagedata" sheetId="10" r:id="rId4"/>
+    <sheet name="Summary" sheetId="4" r:id="rId5"/>
+    <sheet name="H2Heavy, capacities" sheetId="1" r:id="rId6"/>
+    <sheet name="H2Heavy, demands" sheetId="2" r:id="rId7"/>
+    <sheet name="TYNDP2024" sheetId="6" r:id="rId8"/>
+    <sheet name="Eurostat" sheetId="5" r:id="rId9"/>
+    <sheet name="source" sheetId="3" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">storagedata!$A$1:$F$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="128">
   <si>
     <t>Country</t>
   </si>
@@ -435,6 +439,21 @@
   </si>
   <si>
     <t>unit_name_prefix</t>
+  </si>
+  <si>
+    <t>upwardLimit</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>balancePenalty</t>
+  </si>
+  <si>
+    <t>selfDischargeLoss</t>
+  </si>
+  <si>
+    <t>maxSpill</t>
   </si>
 </sst>
 </file>
@@ -446,7 +465,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.##########"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +569,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -718,7 +744,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -848,6 +874,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,7 +894,7 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{B922DAB1-96BE-4C47-ACB7-A4E9C8932980}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -876,6 +915,55 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1130,18 +1218,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20DC892E-7082-4467-928B-8F4B2C671031}" name="Table1" displayName="Table1" ref="A1:I28" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{53CAE17E-E130-454C-A23D-D1F2C5367D34}" name="Table2" displayName="Table2" ref="A1:J22" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:J22" xr:uid="{618B6211-7040-488C-9F85-846A32BD1FFB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J22">
+    <sortCondition ref="B1:B22"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{FD66C488-929A-4E40-97B9-698BE28209C7}" name="Country" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{04387B0B-A6A1-47CC-82EB-6B34AE82821B}" name="Grid"/>
+    <tableColumn id="3" xr3:uid="{57483FE3-C6A9-426F-9DF7-4926168CE122}" name="Node_suffix"/>
+    <tableColumn id="4" xr3:uid="{F155858A-1910-4203-8242-FCFC753CE0F1}" name="Scenario" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{2976D6D8-21B5-4358-9605-474352CC3FAF}" name="Year" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{894F3647-7759-4FB2-B8B6-24582E443654}" name="upwardLimit" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{622B05A3-F0D0-4BEE-B5E5-8AA1239444AE}" name="reference" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{FB556C05-FAE9-43E0-9FC0-D26AB24EC6BC}" name="balancePenalty" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{7EAD7D20-CDA2-446F-BC00-8EC30C32C13B}" name="selfDischargeLoss" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{078F1241-6AF8-480F-897B-1DA7DB1520F6}" name="maxSpill" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20DC892E-7082-4467-928B-8F4B2C671031}" name="Table1" displayName="Table1" ref="A1:I28" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A1:I28" xr:uid="{20DC892E-7082-4467-928B-8F4B2C671031}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{90B3BA90-E856-467E-A12E-718C92D72014}" name="Country" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{47E364C8-C977-4369-A805-4B42B4F3422D}" name="Generator_ID" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{D50F5294-47D2-4C56-800B-3E44FF430FA7}" name="Scenario" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{649C99FE-77E1-437E-9EDE-D888843F1482}" name="Year" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{1A49AF74-6C24-40D6-B37A-D2ADAB4DE02B}" name="capacity_input1" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{F30D702A-E7C4-4705-81A5-A391EA397049}" name="capacity_output1" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{B74AC38E-95FA-433D-B521-50231B26F101}" name="node_suffix_output2" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{2E1D1700-DA32-4625-8DFD-E756415F2202}" name="capacity_output2" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{89275BD6-4B5C-4E77-BA1F-FF40DDEF4E2A}" name="Note" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{90B3BA90-E856-467E-A12E-718C92D72014}" name="Country" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{47E364C8-C977-4369-A805-4B42B4F3422D}" name="Generator_ID" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{D50F5294-47D2-4C56-800B-3E44FF430FA7}" name="Scenario" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{649C99FE-77E1-437E-9EDE-D888843F1482}" name="Year" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{1A49AF74-6C24-40D6-B37A-D2ADAB4DE02B}" name="capacity_input1" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{F30D702A-E7C4-4705-81A5-A391EA397049}" name="capacity_output1" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{B74AC38E-95FA-433D-B521-50231B26F101}" name="node_suffix_output2" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{2E1D1700-DA32-4625-8DFD-E756415F2202}" name="capacity_output2" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{89275BD6-4B5C-4E77-BA1F-FF40DDEF4E2A}" name="Note" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2628,6 +2738,26 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B09C0C-DE72-4694-9C81-3F315378B707}">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DC1340-3E97-4D2C-954C-BCE3B932444C}">
   <sheetPr>
@@ -2635,7 +2765,7 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
@@ -2942,7 +3072,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D2" sqref="D2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,6 +3541,543 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5A18FE-1243-432E-8A1A-21317EE02799}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="58"/>
+    <col min="2" max="3" width="19.7109375" style="58" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="60"/>
+    <col min="6" max="6" width="16.7109375" style="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="63" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="63" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="63" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="63" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5703125" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" s="62" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="66">
+        <v>1</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="60">
+        <v>1</v>
+      </c>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="60">
+        <v>1</v>
+      </c>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="60">
+        <v>1</v>
+      </c>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="60">
+        <v>1</v>
+      </c>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="60">
+        <v>1</v>
+      </c>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="60">
+        <v>1</v>
+      </c>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="60">
+        <v>1</v>
+      </c>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="60">
+        <v>1</v>
+      </c>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="60">
+        <v>1</v>
+      </c>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="60">
+        <v>1</v>
+      </c>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="60">
+        <v>1</v>
+      </c>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="60">
+        <v>1</v>
+      </c>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="60">
+        <v>1</v>
+      </c>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="60">
+        <v>1</v>
+      </c>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="60">
+        <v>1</v>
+      </c>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="60">
+        <v>1</v>
+      </c>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="60">
+        <v>1</v>
+      </c>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="60">
+        <v>1</v>
+      </c>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="60">
+        <v>1</v>
+      </c>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67">
+        <v>4000</v>
+      </c>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="63"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942E5AC9-3C1B-4FDD-828A-AC7EBE9C8D91}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -5518,7 +6185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -6313,7 +6980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87F8DD7-3640-46A5-BBAB-0B6256890B28}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -6646,7 +7313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21420AE7-C1DE-45D2-B734-1504B0A55513}">
   <dimension ref="A1:D42"/>
   <sheetViews>
@@ -7250,7 +7917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF1E2CA-F2CE-4C62-89A9-2315CD87B914}">
   <dimension ref="A2:Q60"/>
   <sheetViews>
@@ -9738,24 +10405,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B09C0C-DE72-4694-9C81-3F315378B707}">
-  <dimension ref="B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>